<commit_message>
Approval Process Test Case addition
</commit_message>
<xml_diff>
--- a/ORIMSproject/src/test/resources/testdata/testdata.xlsx
+++ b/ORIMSproject/src/test/resources/testdata/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sheli\git\main\ORIMSproject\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EF8895A-8611-48A2-9DE2-463A5771289D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84BCC357-A5D7-48EF-8147-590634FDC731}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Section2" sheetId="3" r:id="rId3"/>
     <sheet name="Section3" sheetId="4" r:id="rId4"/>
     <sheet name="Section4" sheetId="5" r:id="rId5"/>
+    <sheet name="chequeDetails" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="47">
   <si>
     <t>username</t>
   </si>
@@ -82,88 +83,94 @@
     <t>File Received Date</t>
   </si>
   <si>
+    <t>Western</t>
+  </si>
+  <si>
+    <t>Colombo</t>
+  </si>
+  <si>
+    <t>Choose Tuesday, October 29th, 2024</t>
+  </si>
+  <si>
+    <t>Choose Monday, November 18th, 2024</t>
+  </si>
+  <si>
+    <t>Dehiwala</t>
+  </si>
+  <si>
+    <t>Dehiwala West</t>
+  </si>
+  <si>
+    <t>Applicant Type</t>
+  </si>
+  <si>
+    <t>Applicant Title</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Relationship</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Full Name</t>
+  </si>
+  <si>
+    <t>Mr</t>
+  </si>
+  <si>
+    <t>Marital Status</t>
+  </si>
+  <si>
+    <t>Complaint Date</t>
+  </si>
+  <si>
+    <t>Kapila</t>
+  </si>
+  <si>
+    <t>Married</t>
+  </si>
+  <si>
+    <t>456785432v</t>
+  </si>
+  <si>
+    <t>Place</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>CompensationValue</t>
+  </si>
+  <si>
+    <t>Applicant</t>
+  </si>
+  <si>
+    <t>Spouse</t>
+  </si>
+  <si>
+    <t>Harsha</t>
+  </si>
+  <si>
+    <t>698973567v</t>
+  </si>
+  <si>
     <t>Allocate</t>
   </si>
   <si>
-    <t>Western</t>
-  </si>
-  <si>
-    <t>Colombo</t>
-  </si>
-  <si>
     <t>Amanda User</t>
   </si>
   <si>
-    <t>Choose Tuesday, October 29th, 2024</t>
-  </si>
-  <si>
-    <t>Choose Monday, November 18th, 2024</t>
-  </si>
-  <si>
-    <t>Dehiwala</t>
-  </si>
-  <si>
-    <t>Dehiwala West</t>
-  </si>
-  <si>
-    <t>Kalpa</t>
-  </si>
-  <si>
-    <t>568974567v</t>
-  </si>
-  <si>
-    <t>Applicant Type</t>
-  </si>
-  <si>
-    <t>Applicant Title</t>
-  </si>
-  <si>
-    <t>Address</t>
-  </si>
-  <si>
-    <t>Relationship</t>
-  </si>
-  <si>
-    <t>Title</t>
-  </si>
-  <si>
-    <t>Full Name</t>
-  </si>
-  <si>
-    <t>Mr</t>
-  </si>
-  <si>
-    <t>Father</t>
-  </si>
-  <si>
-    <t>Marital Status</t>
-  </si>
-  <si>
-    <t>Complaint Date</t>
-  </si>
-  <si>
-    <t>Kapila</t>
-  </si>
-  <si>
-    <t>Married</t>
-  </si>
-  <si>
-    <t>456785432v</t>
-  </si>
-  <si>
-    <t>Choose wednesday, October 30th, 2024</t>
-  </si>
-  <si>
-    <t>Place</t>
-  </si>
-  <si>
-    <t>Test</t>
-  </si>
-  <si>
-    <t>CompensationValue</t>
-  </si>
-  <si>
-    <t>Applicant</t>
+    <t>VoucherNumber</t>
+  </si>
+  <si>
+    <t>Cheque Number</t>
+  </si>
+  <si>
+    <t>Issued Date</t>
   </si>
 </sst>
 </file>
@@ -591,8 +598,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8B71644-83CE-43CB-94C4-40DCCE9185C9}">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -648,7 +655,7 @@
         <v>16</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -662,34 +669,34 @@
         <v>14</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>23</v>
-      </c>
       <c r="J2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="M2" t="s">
         <v>20</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -709,7 +716,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -722,30 +729,30 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -756,10 +763,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D4B3640-83E1-4E18-B550-42E555B0173B}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -773,70 +780,77 @@
     <col min="8" max="8" width="14.6640625" customWidth="1"/>
     <col min="9" max="9" width="13.21875" customWidth="1"/>
     <col min="10" max="10" width="32.88671875" customWidth="1"/>
+    <col min="11" max="11" width="33.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="A1" s="6" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D1" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="K1" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="J1" s="3" t="s">
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I2" t="s">
-        <v>42</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>40</v>
+      <c r="K2" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -849,7 +863,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -860,27 +874,27 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="9" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
         <v>33</v>
       </c>
-      <c r="B2" t="s">
-        <v>38</v>
-      </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2">
         <v>100</v>
@@ -889,4 +903,47 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57FD1836-721E-4F81-AFBD-63F38CB48A59}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="18.21875" customWidth="1"/>
+    <col min="2" max="2" width="14.77734375" customWidth="1"/>
+    <col min="3" max="3" width="32.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>45678326</v>
+      </c>
+      <c r="B2">
+        <v>567890</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
GPC and Log write update
</commit_message>
<xml_diff>
--- a/ORIMSproject/src/test/resources/testdata/testdata.xlsx
+++ b/ORIMSproject/src/test/resources/testdata/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sheli\git\main\ORIMSproject\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84BCC357-A5D7-48EF-8147-590634FDC731}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{315CF7E0-B3A5-49C2-A1DD-78B8167A0492}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,6 +19,7 @@
     <sheet name="Section3" sheetId="4" r:id="rId4"/>
     <sheet name="Section4" sheetId="5" r:id="rId5"/>
     <sheet name="chequeDetails" sheetId="6" r:id="rId6"/>
+    <sheet name="chequePrint" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="53">
   <si>
     <t>username</t>
   </si>
@@ -89,12 +90,6 @@
     <t>Colombo</t>
   </si>
   <si>
-    <t>Choose Tuesday, October 29th, 2024</t>
-  </si>
-  <si>
-    <t>Choose Monday, November 18th, 2024</t>
-  </si>
-  <si>
     <t>Dehiwala</t>
   </si>
   <si>
@@ -171,6 +166,30 @@
   </si>
   <si>
     <t>Issued Date</t>
+  </si>
+  <si>
+    <t>786567865v</t>
+  </si>
+  <si>
+    <t>Payment Date</t>
+  </si>
+  <si>
+    <t>Reference No</t>
+  </si>
+  <si>
+    <t>Officer</t>
+  </si>
+  <si>
+    <t>Cheque Officer</t>
+  </si>
+  <si>
+    <t>Choose Sunday, December 1st, 2024</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>Sinhala</t>
   </si>
 </sst>
 </file>
@@ -232,7 +251,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -257,6 +276,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -270,7 +295,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -285,6 +310,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -598,8 +624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8B71644-83CE-43CB-94C4-40DCCE9185C9}">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -655,7 +681,7 @@
         <v>16</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -669,13 +695,13 @@
         <v>14</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>19</v>
+        <v>50</v>
       </c>
       <c r="E2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G2" t="s">
         <v>17</v>
@@ -684,23 +710,61 @@
         <v>18</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" t="s">
         <v>20</v>
       </c>
-      <c r="L2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
-      <c r="D3" s="2"/>
+      <c r="K3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="4" spans="1:13">
       <c r="D4" s="2"/>
@@ -729,30 +793,30 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="D1" s="7" t="s">
         <v>24</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
         <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -766,7 +830,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -785,19 +849,19 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>8</v>
@@ -812,24 +876,24 @@
         <v>11</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s">
         <v>32</v>
       </c>
-      <c r="C2" t="s">
-        <v>34</v>
-      </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E2" t="s">
         <v>18</v>
@@ -841,16 +905,16 @@
         <v>18</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>20</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -874,24 +938,24 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s">
         <v>18</v>
@@ -910,7 +974,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -922,28 +986,76 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>45678326</v>
+        <v>8977787</v>
       </c>
       <c r="B2">
-        <v>567890</v>
+        <v>877676</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>20</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4062CEF4-23FC-41F0-A432-A34E6B0926FE}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="12.33203125" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2">
+        <v>678995</v>
+      </c>
+      <c r="D2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>